<commit_message>
Updated spent 1 log
</commit_message>
<xml_diff>
--- a/Sprint_Docs/Sprint1/Sprint1.xlsx
+++ b/Sprint_Docs/Sprint1/Sprint1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26124"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shubhamgupta/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AlanLi/Desktop/Software Engineering/IC3/Sprint_Docs/Sprint1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14260" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Sprint 1 Burndown" sheetId="5" r:id="rId6"/>
     <sheet name="Action Items" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1561,6 +1561,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1737,28 +1738,28 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>224.0</c:v>
+                  <c:v>258.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>196.0</c:v>
+                  <c:v>225.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>168.0</c:v>
+                  <c:v>193.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>140.0</c:v>
+                  <c:v>161.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>112.0</c:v>
+                  <c:v>129.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>84.0</c:v>
+                  <c:v>96.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.0</c:v>
+                  <c:v>64.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28.0</c:v>
+                  <c:v>32.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.0</c:v>
@@ -1775,11 +1776,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2051286336"/>
-        <c:axId val="-2142873184"/>
+        <c:axId val="-2084275808"/>
+        <c:axId val="-2140634592"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-2051286336"/>
+        <c:axId val="-2084275808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1801,6 +1802,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1817,7 +1819,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2142873184"/>
+        <c:crossAx val="-2140634592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1825,7 +1827,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2142873184"/>
+        <c:axId val="-2140634592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1856,6 +1858,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1877,7 +1880,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2051286336"/>
+        <c:crossAx val="-2084275808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1889,6 +1892,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13198,9 +13202,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T992"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView zoomScale="107" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13391,8 +13395,8 @@
       <c r="D6" s="42" t="s">
         <v>174</v>
       </c>
-      <c r="E6" s="48" t="s">
-        <v>181</v>
+      <c r="E6" s="47" t="s">
+        <v>185</v>
       </c>
       <c r="F6" s="43" t="s">
         <v>184</v>
@@ -13431,7 +13435,7 @@
         <v>110</v>
       </c>
       <c r="B7" s="42">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C7" s="42" t="s">
         <v>62</v>
@@ -13479,7 +13483,7 @@
         <v>143</v>
       </c>
       <c r="B8" s="42">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C8" s="42" t="s">
         <v>62</v>
@@ -13571,7 +13575,7 @@
         <v>114</v>
       </c>
       <c r="B10" s="42">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C10" s="42" t="s">
         <v>62</v>
@@ -13617,7 +13621,7 @@
         <v>116</v>
       </c>
       <c r="B11" s="42">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C11" s="42" t="s">
         <v>62</v>
@@ -13663,7 +13667,7 @@
         <v>117</v>
       </c>
       <c r="B12" s="42">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C12" s="42" t="s">
         <v>62</v>
@@ -13755,7 +13759,7 @@
         <v>136</v>
       </c>
       <c r="B14" s="42">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C14" s="42" t="s">
         <v>62</v>
@@ -14142,7 +14146,7 @@
       </c>
       <c r="B23" s="62">
         <f>SUM(B5:B22)</f>
-        <v>224</v>
+        <v>258</v>
       </c>
       <c r="C23" s="63"/>
       <c r="D23" s="63"/>
@@ -30677,8 +30681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -30840,35 +30844,35 @@
       </c>
       <c r="B6" s="27">
         <f>SUM('Sprint 1'!$B$5:$B$21)-(((B4-1)*SUM('Sprint 1'!$B$5:$B$21))/($J$4-1))</f>
-        <v>224</v>
+        <v>258</v>
       </c>
       <c r="C6" s="28">
         <f>SUM('Sprint 1'!$B$5:$B$21)-(((C4-1)*SUM('Sprint 1'!$B$5:$B$21))/($J$4-1))</f>
-        <v>196</v>
+        <v>225.75</v>
       </c>
       <c r="D6" s="29">
         <f>SUM('Sprint 1'!$B$5:$B$21)-(((D4-1)*SUM('Sprint 1'!$B$5:$B$21))/($J$4-1))</f>
-        <v>168</v>
+        <v>193.5</v>
       </c>
       <c r="E6" s="27">
         <f>SUM('Sprint 1'!$B$5:$B$21)-(((E4-1)*SUM('Sprint 1'!$B$5:$B$21))/($J$4-1))</f>
-        <v>140</v>
+        <v>161.25</v>
       </c>
       <c r="F6" s="28">
         <f>SUM('Sprint 1'!$B$5:$B$21)-(((F4-1)*SUM('Sprint 1'!$B$5:$B$21))/($J$4-1))</f>
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="G6" s="29">
         <f>SUM('Sprint 1'!$B$5:$B$21)-(((G4-1)*SUM('Sprint 1'!$B$5:$B$21))/($J$4-1))</f>
-        <v>84</v>
+        <v>96.75</v>
       </c>
       <c r="H6" s="27">
         <f>SUM('Sprint 1'!$B$5:$B$21)-(((H4-1)*SUM('Sprint 1'!$B$5:$B$21))/($J$4-1))</f>
-        <v>56</v>
+        <v>64.5</v>
       </c>
       <c r="I6" s="28">
         <f>SUM('Sprint 1'!$B$5:$B$21)-(((I4-1)*SUM('Sprint 1'!$B$5:$B$21))/($J$4-1))</f>
-        <v>28</v>
+        <v>32.25</v>
       </c>
       <c r="J6" s="29">
         <f>SUM('Sprint 1'!$B$5:$B$21)-(((J4-1)*SUM('Sprint 1'!$B$5:$B$21))/($J$4-1))</f>

</xml_diff>